<commit_message>
Turn keyword from absetn to abs.
</commit_message>
<xml_diff>
--- a/code/files/ENSTA_sports_test_multi.xlsx
+++ b/code/files/ENSTA_sports_test_multi.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\uni\Sport\System detection d'absences\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\uni\Sport\Absences_sport\code\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{356431E2-3AB9-4F8D-AE9F-3BDAFD7BDA07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00D43B7E-2750-4E47-843B-EBEB9CBC223B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fitness" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="41">
   <si>
     <t>Nom</t>
   </si>
@@ -139,6 +139,15 @@
   </si>
   <si>
     <t>marounjassaf@gmail.com</t>
+  </si>
+  <si>
+    <t>Groupe</t>
+  </si>
+  <si>
+    <t>1A</t>
+  </si>
+  <si>
+    <t>Abs.</t>
   </si>
 </sst>
 </file>
@@ -489,108 +498,111 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q6"/>
+  <dimension ref="A1:R6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="22.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="17" width="10" customWidth="1"/>
+    <col min="2" max="3" width="14" customWidth="1"/>
+    <col min="4" max="4" width="22.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="18" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
         <v>17</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>18</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>19</v>
       </c>
-      <c r="D2" t="s">
-        <v>20</v>
-      </c>
       <c r="E2" t="s">
         <v>20</v>
       </c>
       <c r="F2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" t="s">
         <v>22</v>
       </c>
-      <c r="I2" t="s">
-        <v>20</v>
-      </c>
       <c r="J2" t="s">
         <v>20</v>
       </c>
       <c r="K2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M2" t="s">
         <v>20</v>
@@ -604,28 +616,31 @@
       <c r="P2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="Q2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" t="s">
         <v>23</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>24</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>25</v>
       </c>
-      <c r="D3" t="s">
-        <v>20</v>
-      </c>
       <c r="E3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F3" t="s">
         <v>21</v>
       </c>
       <c r="G3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H3" t="s">
         <v>20</v>
@@ -646,10 +661,10 @@
         <v>20</v>
       </c>
       <c r="N3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="P3" t="s">
         <v>20</v>
@@ -657,20 +672,23 @@
       <c r="Q3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" t="s">
         <v>26</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>27</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>28</v>
       </c>
-      <c r="D4" t="s">
-        <v>20</v>
-      </c>
       <c r="E4" t="s">
         <v>20</v>
       </c>
@@ -710,20 +728,23 @@
       <c r="Q4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" t="s">
         <v>29</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>30</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>31</v>
       </c>
-      <c r="D5" t="s">
-        <v>21</v>
-      </c>
       <c r="E5" t="s">
         <v>21</v>
       </c>
@@ -731,19 +752,19 @@
         <v>21</v>
       </c>
       <c r="G5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" t="s">
         <v>22</v>
       </c>
-      <c r="I5" t="s">
-        <v>20</v>
-      </c>
       <c r="J5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L5" t="s">
         <v>20</v>
@@ -763,20 +784,23 @@
       <c r="Q5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" t="s">
         <v>35</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D6" t="s">
-        <v>20</v>
-      </c>
       <c r="E6" t="s">
         <v>20</v>
       </c>
@@ -787,10 +811,10 @@
         <v>20</v>
       </c>
       <c r="H6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J6" t="s">
         <v>20</v>
@@ -802,10 +826,10 @@
         <v>20</v>
       </c>
       <c r="M6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="O6" t="s">
         <v>20</v>
@@ -814,12 +838,15 @@
         <v>20</v>
       </c>
       <c r="Q6" t="s">
+        <v>20</v>
+      </c>
+      <c r="R6" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C6" r:id="rId1" xr:uid="{D8348E57-D7A5-4E62-83C1-9B9B8614C9B0}"/>
+    <hyperlink ref="D6" r:id="rId1" xr:uid="{D8348E57-D7A5-4E62-83C1-9B9B8614C9B0}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -827,105 +854,110 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Q6"/>
+  <dimension ref="A1:R6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="14" customWidth="1"/>
-    <col min="4" max="17" width="10" customWidth="1"/>
+    <col min="2" max="4" width="14" customWidth="1"/>
+    <col min="5" max="18" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
         <v>17</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>18</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>19</v>
       </c>
-      <c r="D2" t="s">
-        <v>20</v>
-      </c>
       <c r="E2" t="s">
         <v>20</v>
       </c>
       <c r="F2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" t="s">
         <v>22</v>
       </c>
-      <c r="I2" t="s">
-        <v>20</v>
-      </c>
       <c r="J2" t="s">
         <v>20</v>
       </c>
       <c r="K2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M2" t="s">
         <v>20</v>
@@ -939,28 +971,31 @@
       <c r="P2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="Q2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" t="s">
         <v>23</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>24</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>25</v>
       </c>
-      <c r="D3" t="s">
-        <v>20</v>
-      </c>
       <c r="E3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F3" t="s">
         <v>21</v>
       </c>
       <c r="G3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H3" t="s">
         <v>20</v>
@@ -981,10 +1016,10 @@
         <v>20</v>
       </c>
       <c r="N3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="P3" t="s">
         <v>20</v>
@@ -992,20 +1027,23 @@
       <c r="Q3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" t="s">
         <v>26</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>27</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>28</v>
       </c>
-      <c r="D4" t="s">
-        <v>20</v>
-      </c>
       <c r="E4" t="s">
         <v>20</v>
       </c>
@@ -1045,20 +1083,23 @@
       <c r="Q4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" t="s">
         <v>29</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>30</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>31</v>
       </c>
-      <c r="D5" t="s">
-        <v>21</v>
-      </c>
       <c r="E5" t="s">
         <v>21</v>
       </c>
@@ -1066,19 +1107,19 @@
         <v>21</v>
       </c>
       <c r="G5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" t="s">
         <v>22</v>
       </c>
-      <c r="I5" t="s">
-        <v>20</v>
-      </c>
       <c r="J5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L5" t="s">
         <v>20</v>
@@ -1098,20 +1139,23 @@
       <c r="Q5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" t="s">
         <v>32</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>33</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>34</v>
       </c>
-      <c r="D6" t="s">
-        <v>20</v>
-      </c>
       <c r="E6" t="s">
         <v>20</v>
       </c>
@@ -1122,10 +1166,10 @@
         <v>20</v>
       </c>
       <c r="H6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J6" t="s">
         <v>20</v>
@@ -1137,10 +1181,10 @@
         <v>20</v>
       </c>
       <c r="M6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="O6" t="s">
         <v>20</v>
@@ -1149,6 +1193,9 @@
         <v>20</v>
       </c>
       <c r="Q6" t="s">
+        <v>20</v>
+      </c>
+      <c r="R6" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1159,105 +1206,111 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Q6"/>
+  <dimension ref="A1:R6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="14" customWidth="1"/>
-    <col min="4" max="17" width="10" customWidth="1"/>
+    <col min="2" max="3" width="14" customWidth="1"/>
+    <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="18" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
         <v>17</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>18</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>19</v>
       </c>
-      <c r="D2" t="s">
-        <v>20</v>
-      </c>
       <c r="E2" t="s">
         <v>20</v>
       </c>
       <c r="F2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G2" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="H2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" t="s">
         <v>22</v>
       </c>
-      <c r="I2" t="s">
-        <v>20</v>
-      </c>
       <c r="J2" t="s">
         <v>20</v>
       </c>
       <c r="K2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L2" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="M2" t="s">
         <v>20</v>
@@ -1271,28 +1324,31 @@
       <c r="P2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="Q2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" t="s">
         <v>23</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>24</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>25</v>
       </c>
-      <c r="D3" t="s">
-        <v>20</v>
-      </c>
       <c r="E3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F3" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="G3" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="H3" t="s">
         <v>20</v>
@@ -1313,10 +1369,10 @@
         <v>20</v>
       </c>
       <c r="N3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O3" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="P3" t="s">
         <v>20</v>
@@ -1324,20 +1380,23 @@
       <c r="Q3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" t="s">
         <v>26</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>27</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>28</v>
       </c>
-      <c r="D4" t="s">
-        <v>20</v>
-      </c>
       <c r="E4" t="s">
         <v>20</v>
       </c>
@@ -1377,40 +1436,43 @@
       <c r="Q4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" t="s">
         <v>29</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>30</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>31</v>
       </c>
-      <c r="D5" t="s">
-        <v>21</v>
-      </c>
       <c r="E5" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="F5" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="G5" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="H5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" t="s">
         <v>22</v>
       </c>
-      <c r="I5" t="s">
-        <v>20</v>
-      </c>
       <c r="J5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K5" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="L5" t="s">
         <v>20</v>
@@ -1430,20 +1492,23 @@
       <c r="Q5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" t="s">
         <v>32</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>33</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>34</v>
       </c>
-      <c r="D6" t="s">
-        <v>20</v>
-      </c>
       <c r="E6" t="s">
         <v>20</v>
       </c>
@@ -1454,10 +1519,10 @@
         <v>20</v>
       </c>
       <c r="H6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I6" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="J6" t="s">
         <v>20</v>
@@ -1469,10 +1534,10 @@
         <v>20</v>
       </c>
       <c r="M6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N6" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="O6" t="s">
         <v>20</v>
@@ -1481,6 +1546,9 @@
         <v>20</v>
       </c>
       <c r="Q6" t="s">
+        <v>20</v>
+      </c>
+      <c r="R6" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>